<commit_message>
tab1d => 2d fini, début colorisation
il reste la colorisation des cellules et le tri éventuel des colonnes
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -374,21 +374,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:9">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -396,15 +393,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>80</v>
       </c>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>4</v>
       </c>

</xml_diff>